<commit_message>
#30-Introduced columns payment method and type of outlet in Daily Summarize Transactions Report
</commit_message>
<xml_diff>
--- a/Beelina.API/Templates/ReportTemplates/DailySummarizeTransactionsReport_Template.xlsx
+++ b/Beelina.API/Templates/ReportTemplates/DailySummarizeTransactionsReport_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Beelina\Beelina.API\Templates\ReportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80082F7-EC51-4A74-B5E5-375560EB4500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7629720-6813-4053-87D4-733B394C239C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E4D0BD8-5D1B-4F5A-A703-D8DC3D2DB4A5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Current Stocks</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>Collectibles (Not Paid)</t>
+  </si>
+  <si>
+    <t>Type of Outlet</t>
+  </si>
+  <si>
+    <t>Payment Method</t>
   </si>
 </sst>
 </file>
@@ -439,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{598EC0B1-1341-425D-9BC5-21A9B57CB7DB}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,13 +460,15 @@
     <col min="5" max="5" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -471,12 +479,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -499,17 +507,23 @@
         <v>6</v>
       </c>
       <c r="H4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="3"/>
+      <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="K6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -517,18 +531,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -714,6 +728,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E8796B7-9C8F-49E2-8465-EBA71059CE19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{055FEFB9-C360-4F39-AAB4-B29E8525E846}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -725,14 +747,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E8796B7-9C8F-49E2-8465-EBA71059CE19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
#35-Introduced product price per panel
</commit_message>
<xml_diff>
--- a/Beelina.API/Templates/ReportTemplates/DailySummarizeTransactionsReport_Template.xlsx
+++ b/Beelina.API/Templates/ReportTemplates/DailySummarizeTransactionsReport_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Beelina\Beelina.API\Templates\ReportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7629720-6813-4053-87D4-733B394C239C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C0F9EE-616E-4DBD-8083-9AD81092C498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E4D0BD8-5D1B-4F5A-A703-D8DC3D2DB4A5}"/>
   </bookViews>
@@ -38,12 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t>Current Stocks</t>
-  </si>
-  <si>
-    <t>After Stocks</t>
-  </si>
-  <si>
     <t>Total Sales</t>
   </si>
   <si>
@@ -75,6 +69,12 @@
   </si>
   <si>
     <t>Payment Method</t>
+  </si>
+  <si>
+    <t>Initial Stocks Value</t>
+  </si>
+  <si>
+    <t>Remaining Stocks Value</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,13 +470,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -486,34 +486,34 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="K4" s="3"/>
     </row>
@@ -531,18 +531,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -728,14 +728,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E8796B7-9C8F-49E2-8465-EBA71059CE19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{055FEFB9-C360-4F39-AAB4-B29E8525E846}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -747,6 +739,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E8796B7-9C8F-49E2-8465-EBA71059CE19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
#43-Calculate discount amount on Daily Summarize Transaction Report.
</commit_message>
<xml_diff>
--- a/Beelina.API/Templates/ReportTemplates/DailySummarizeTransactionsReport_Template.xlsx
+++ b/Beelina.API/Templates/ReportTemplates/DailySummarizeTransactionsReport_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Beelina\Beelina.API\Templates\ReportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C0F9EE-616E-4DBD-8083-9AD81092C498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940CAE2A-F763-4E43-9F76-F93AFBB33289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E4D0BD8-5D1B-4F5A-A703-D8DC3D2DB4A5}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Total Sales</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Store Name</t>
   </si>
@@ -53,18 +50,12 @@
     <t>Area Covered</t>
   </si>
   <si>
-    <t>Discounts given per store</t>
-  </si>
-  <si>
     <t>Order Received (Date)</t>
   </si>
   <si>
     <t>Due Collectibles (Deadline)</t>
   </si>
   <si>
-    <t>Collectibles (Not Paid)</t>
-  </si>
-  <si>
     <t>Type of Outlet</t>
   </si>
   <si>
@@ -75,6 +66,27 @@
   </si>
   <si>
     <t>Remaining Stocks Value</t>
+  </si>
+  <si>
+    <t>Total Gross Sales</t>
+  </si>
+  <si>
+    <t>Discount Amount</t>
+  </si>
+  <si>
+    <t>Total Net Sales</t>
+  </si>
+  <si>
+    <t>Gross Collectibles</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>Discounted Collectibles</t>
+  </si>
+  <si>
+    <t>Net Collectibles</t>
   </si>
 </sst>
 </file>
@@ -118,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -131,6 +143,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,85 +464,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{598EC0B1-1341-425D-9BC5-21A9B57CB7DB}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="K5" s="1"/>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="8"/>
+      <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="K6" s="1"/>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="J6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -531,18 +562,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -728,6 +759,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E8796B7-9C8F-49E2-8465-EBA71059CE19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{055FEFB9-C360-4F39-AAB4-B29E8525E846}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -739,14 +778,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E8796B7-9C8F-49E2-8465-EBA71059CE19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>